<commit_message>
more vendor class added from py2 to py3
</commit_message>
<xml_diff>
--- a/csv/outfile/vendor_ids.xlsx
+++ b/csv/outfile/vendor_ids.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berries\Code\csv\outfile\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="vendor_ids" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="798">
   <si>
     <t>ids</t>
   </si>
@@ -2410,6 +2405,9 @@
   </si>
   <si>
     <t>Papas_Candle_Shoppe_8077.xls</t>
+  </si>
+  <si>
+    <t>Peaceful_Village_Jewelry_SHST.xls</t>
   </si>
 </sst>
 </file>
@@ -2979,7 +2977,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3014,7 +3012,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3191,7 +3189,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3201,8 +3199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4562,6 +4560,9 @@
       <c r="G57" t="s">
         <v>340</v>
       </c>
+      <c r="H57" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">

</xml_diff>

<commit_message>
more vendor class added from py 2 to 3
</commit_message>
<xml_diff>
--- a/csv/outfile/vendor_ids.xlsx
+++ b/csv/outfile/vendor_ids.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="13440"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="13530" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="vendor_ids" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="806">
   <si>
     <t>ids</t>
   </si>
@@ -2408,6 +2408,30 @@
   </si>
   <si>
     <t>Peaceful_Village_Jewelry_SHST.xls</t>
+  </si>
+  <si>
+    <t>Shoots Roots &amp; Leather Boots</t>
+  </si>
+  <si>
+    <t>Shoots_Roots_&amp;_Leather_Boots</t>
+  </si>
+  <si>
+    <t>Shoots_Roots_&amp;_Leather_Boots_8116.xls</t>
+  </si>
+  <si>
+    <t>potpourri160</t>
+  </si>
+  <si>
+    <t>potpourri400</t>
+  </si>
+  <si>
+    <t>potpourri800</t>
+  </si>
+  <si>
+    <t>Shoots_Roots_&amp;_Leather_Boots_shst.xls</t>
+  </si>
+  <si>
+    <t>Shoots_Roots_&amp;_Leather_Boots_buyhere.xlsx</t>
   </si>
 </sst>
 </file>
@@ -3189,7 +3213,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3197,10 +3221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6266,7 +6290,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>8069</v>
       </c>
@@ -6289,7 +6313,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>8070</v>
       </c>
@@ -6312,7 +6336,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>8071</v>
       </c>
@@ -6338,7 +6362,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>8072</v>
       </c>
@@ -6364,7 +6388,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>8073</v>
       </c>
@@ -6387,7 +6411,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>8074</v>
       </c>
@@ -6413,7 +6437,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>8076</v>
       </c>
@@ -6439,7 +6463,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>8077</v>
       </c>
@@ -6456,9 +6480,33 @@
         <v>796</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>8078</v>
+        <v>8116</v>
+      </c>
+      <c r="B137" t="s">
+        <v>798</v>
+      </c>
+      <c r="C137" t="s">
+        <v>799</v>
+      </c>
+      <c r="D137" t="s">
+        <v>800</v>
+      </c>
+      <c r="E137" t="s">
+        <v>801</v>
+      </c>
+      <c r="F137" t="s">
+        <v>802</v>
+      </c>
+      <c r="G137" t="s">
+        <v>803</v>
+      </c>
+      <c r="H137" t="s">
+        <v>804</v>
+      </c>
+      <c r="I137" t="s">
+        <v>805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>